<commit_message>
add endpoint for User Question
</commit_message>
<xml_diff>
--- a/chatbot.xlsx
+++ b/chatbot.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>what is your name</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>bla bla bla</t>
+  </si>
+  <si>
+    <t>ما اسم مدير يونا</t>
+  </si>
+  <si>
+    <t>عاطف</t>
   </si>
 </sst>
 </file>
@@ -378,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,6 +422,14 @@
       </c>
       <c r="B4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use OpenAPi To get a hand from ai tool
</commit_message>
<xml_diff>
--- a/chatbot.xlsx
+++ b/chatbot.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>what is your name</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>عاطف</t>
+  </si>
+  <si>
+    <t>ما اسمك</t>
+  </si>
+  <si>
+    <t>يونا شات بوت</t>
+  </si>
+  <si>
+    <t>adsf</t>
+  </si>
+  <si>
+    <t>asdf</t>
   </si>
 </sst>
 </file>
@@ -384,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,6 +442,22 @@
       </c>
       <c r="B5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update get_most_similar_question from database to work with fuzz ratio
</commit_message>
<xml_diff>
--- a/chatbot.xlsx
+++ b/chatbot.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581A46AB-2F04-4249-B4BA-6E88F69F6284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>answer</t>
   </si>
@@ -24,28 +25,16 @@
     <t>question</t>
   </si>
   <si>
-    <t>من مدير منظمة التعاون الاسلامي</t>
+    <t>الاستاذ محمد</t>
   </si>
   <si>
-    <t>الاستاذ عاطف</t>
-  </si>
-  <si>
-    <t xml:space="preserve">من انت </t>
-  </si>
-  <si>
-    <t>انا يونا شات بوت</t>
-  </si>
-  <si>
-    <t>من مدير جريدة يونا</t>
-  </si>
-  <si>
-    <t>عاطف</t>
+    <t xml:space="preserve">من رئيس جريدة يونا </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,14 +76,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -132,7 +124,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -204,7 +196,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -377,14 +369,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -396,26 +392,10 @@
     </row>
     <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -424,7 +404,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -436,7 +416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Edit questions from the upload page
</commit_message>
<xml_diff>
--- a/chatbot.xlsx
+++ b/chatbot.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CE43EF-5DE4-47A4-8727-4B8F938F7511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CA160D-0295-4BC1-A1F3-720FC6435DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -322,18 +322,12 @@
     <t>هل يمكنني التبديل بين منتجات مختلفة؟</t>
   </si>
   <si>
-    <t>يمكنك تسجيل الدخول إلى حسابك من خلال صفحة تسجيل الدخول على الموقع الإلكتروني.</t>
-  </si>
-  <si>
     <t>ساعات العمل الخاصة بالشركة هي من الساعة 9 صباحًا حتى الساعة 5 مساءً، من الاثنين إلى الجمعة.</t>
   </si>
   <si>
     <t>نعم، نقدم خدمة العملاء عبر الهاتف. يمكنك الاتصال على الرقم [رقم الهاتف].</t>
   </si>
   <si>
-    <t>يقع مكتبنا الرئيسي في [عنوان المكتب].</t>
-  </si>
-  <si>
     <t>يمكنك استعادة كلمة المرور الخاصة بك من خلال صفحة "نسيت كلمة المرور" على الموقع.</t>
   </si>
   <si>
@@ -616,7 +610,15 @@
     <t>نعم، نقدم خدمة تبديل المنتجات إذا لم تكن راضيًا. اتصل بالدعم لبدء عملية التبديل.</t>
   </si>
   <si>
-    <t>اسمي هو يونا شات بوت .</t>
+    <t>يقع مكتبنا الرئيسي في  السعودية مدينة جده .</t>
+  </si>
+  <si>
+    <t>1-يمكنك تسجيل الدخول إلى حسابك من خلال  صفحة 
+سجيل الدخول على الموقع الإلكتروني-2.
+3- اسلام</t>
+  </si>
+  <si>
+    <t>يونا شات بوت .</t>
   </si>
 </sst>
 </file>
@@ -652,8 +654,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -961,13 +966,12 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="1" max="2" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -986,12 +990,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>101</v>
+      <c r="B3" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -999,7 +1003,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1007,7 +1011,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1015,7 +1019,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1023,7 +1027,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1031,7 +1035,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1039,7 +1043,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1047,7 +1051,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1055,7 +1059,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1063,7 +1067,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1071,7 +1075,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1079,7 +1083,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1087,7 +1091,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1095,7 +1099,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1103,7 +1107,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1111,7 +1115,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1119,7 +1123,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1127,7 +1131,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1135,7 +1139,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1143,7 +1147,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1151,7 +1155,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1159,7 +1163,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1167,7 +1171,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1175,7 +1179,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1183,7 +1187,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1191,7 +1195,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1199,7 +1203,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1207,7 +1211,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1215,7 +1219,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1223,7 +1227,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1231,7 +1235,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1239,7 +1243,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1247,7 +1251,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1255,7 +1259,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1263,7 +1267,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1271,7 +1275,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1279,7 +1283,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1287,7 +1291,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1295,7 +1299,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1303,7 +1307,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1311,7 +1315,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1319,7 +1323,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1327,7 +1331,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1335,7 +1339,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1343,7 +1347,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1351,7 +1355,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1359,7 +1363,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1367,7 +1371,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1375,7 +1379,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1383,7 +1387,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1391,7 +1395,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1399,7 +1403,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1407,7 +1411,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1415,7 +1419,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1423,7 +1427,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1431,7 +1435,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1439,7 +1443,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1447,7 +1451,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1455,7 +1459,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1463,7 +1467,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1471,7 +1475,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1479,7 +1483,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1487,7 +1491,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1495,7 +1499,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1503,7 +1507,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1511,7 +1515,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1519,7 +1523,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1527,7 +1531,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1535,7 +1539,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1543,7 +1547,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1551,7 +1555,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1559,7 +1563,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1567,7 +1571,7 @@
         <v>36</v>
       </c>
       <c r="B75" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1575,7 +1579,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1583,7 +1587,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1591,7 +1595,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1599,7 +1603,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1607,7 +1611,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1615,7 +1619,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1623,7 +1627,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1631,7 +1635,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1639,7 +1643,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1647,7 +1651,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1655,7 +1659,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1663,7 +1667,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1671,7 +1675,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1679,7 +1683,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1687,7 +1691,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1695,7 +1699,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1703,7 +1707,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1711,7 +1715,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1719,7 +1723,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1727,7 +1731,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1735,7 +1739,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1743,7 +1747,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1751,7 +1755,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1759,7 +1763,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1767,7 +1771,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1775,7 +1779,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add unanswerd questions conf
</commit_message>
<xml_diff>
--- a/chatbot.xlsx
+++ b/chatbot.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CA160D-0295-4BC1-A1F3-720FC6435DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B34D27B-8088-4FB7-971F-2F47436C751D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="202">
   <si>
     <t>answer</t>
   </si>
@@ -619,6 +619,12 @@
   </si>
   <si>
     <t>يونا شات بوت .</t>
+  </si>
+  <si>
+    <t>funny_answer</t>
+  </si>
+  <si>
+    <t>fuck</t>
   </si>
 </sst>
 </file>
@@ -963,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,23 +980,29 @@
     <col min="1" max="2" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -998,7 +1010,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1018,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1014,7 +1026,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1022,7 +1034,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1030,7 +1042,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1038,7 +1050,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1046,7 +1058,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1054,7 +1066,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1062,7 +1074,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1070,7 +1082,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1078,7 +1090,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1086,7 +1098,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1094,7 +1106,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>

</xml_diff>